<commit_message>
Updating player + Camera follow
Player can auto follow or stay. Player follow each other and regroup at the destination. Camera follows selected player.
+SCR_MoveCharacter
+Documents Update
</commit_message>
<xml_diff>
--- a/Documents/time schedule.xlsx
+++ b/Documents/time schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Time spend</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Info</t>
-  </si>
-  <si>
     <t>Time (hours)</t>
   </si>
   <si>
@@ -48,13 +45,37 @@
   </si>
   <si>
     <t>Player walk through level, pick player, spawn player, show id above head</t>
+  </si>
+  <si>
+    <t>Camera follow players + switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player following and regrouping when at destination </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characters auto follow or staying </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Info: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>this includes research, coding and testing</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +94,13 @@
       <b/>
       <u/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -516,7 +544,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,10 +567,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -553,7 +581,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -564,7 +592,7 @@
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -575,7 +603,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -586,23 +614,41 @@
         <v>7.6388888888888895E-2</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>43030</v>
+      </c>
+      <c r="B8" s="12">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-    </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="11">
+        <v>43030</v>
+      </c>
+      <c r="B9" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="11">
+        <v>43030</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>

</xml_diff>

<commit_message>
Adding HUD + picking up ammo
HUD + ammo: Added a hud where the 4 players are viewd on. Under the player you can find the active gun with their ammo. You can pick ammo up that lays on the ground. Level update with the new HUD and pickups
+SCR_HUD
+SCR_BulletPickUp

+SCN_Level1

+Pickup_ BulletsHandgun
+Pickup_ BulletsPersuader
+Pickup_ BulletsRifle

+Texture: Bullet
+Texture: Capsule
+Texture: HandGun
+Texture: Persuader
+Texture: Rifle

+M_BulletsGun
+M_BulletsPersuader
+M_BulletsRifle
</commit_message>
<xml_diff>
--- a/Documents/time schedule.xlsx
+++ b/Documents/time schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Time spend</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>When mouse hovers above enemy the cursor change</t>
+  </si>
+  <si>
+    <t>Making HUD + updating HUD script (bullets + active weapon)</t>
+  </si>
+  <si>
+    <t>Pickups bullets</t>
   </si>
 </sst>
 </file>
@@ -693,14 +699,26 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
+      <c r="A14" s="11">
+        <v>43032</v>
+      </c>
+      <c r="B14" s="12">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
+      <c r="A15" s="11">
+        <v>43032</v>
+      </c>
+      <c r="B15" s="12">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>

</xml_diff>

<commit_message>
Updating Inventory: Health + weapons
Inventory update: You can pick up Health and weapons. If you pick up a weapon you dont already have you can use it with switching with mouse scroll wheel. The health is just an example of items you can pickup. Cant use it only pickup and see in the inventory
+SCR_ItemPickUp
+SCR_Medkit

+SCN_Level1

+Pickup_MedKit
+Pickup_Persuader
+Pickup_Rifle

+Texture: Medkit

+M_MedkitGreen
</commit_message>
<xml_diff>
--- a/Documents/time schedule.xlsx
+++ b/Documents/time schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Time spend</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Recreating manager, spawning object in game manager not other class</t>
+  </si>
+  <si>
+    <t>Updating inventory UI showing icon of object.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Picking up weapons(if you don’t have it already) and picking up health + showing in inventory. </t>
   </si>
 </sst>
 </file>
@@ -568,7 +574,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,14 +769,26 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
+      <c r="A19" s="11">
+        <v>43034</v>
+      </c>
+      <c r="B19" s="12">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
+      <c r="A20" s="11">
+        <v>43034</v>
+      </c>
+      <c r="B20" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>

</xml_diff>